<commit_message>
fifth commit - update test cases name
</commit_message>
<xml_diff>
--- a/resources/DataLoginMenu.xlsx
+++ b/resources/DataLoginMenu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/G2Lab/FinalProject/QuotaAppTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E334A5-4611-634B-A04B-351A00C16EAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B9BE18-39CF-5648-BB89-6650443AB045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="111">
   <si>
     <t>password</t>
   </si>
@@ -136,48 +136,9 @@
     <t>positif case - correct phone number and password</t>
   </si>
   <si>
-    <t>negative case - wrong password</t>
-  </si>
-  <si>
-    <t>negative case - wrong phone number</t>
-  </si>
-  <si>
-    <t>negative case - wrong phone number and password</t>
-  </si>
-  <si>
     <t>+628123456789101112</t>
   </si>
   <si>
-    <t>negative case - wrong phone number (outside Indonesia)</t>
-  </si>
-  <si>
-    <t>negative case - wrong phone number format (exceed 12 characters)</t>
-  </si>
-  <si>
-    <t>negative case - wrong phone number format (not numerical)</t>
-  </si>
-  <si>
-    <t>negative case - wrong phone number (unregistered number)</t>
-  </si>
-  <si>
-    <t>negative case - wrong phone number (unverified number)</t>
-  </si>
-  <si>
-    <t>negative case - wrong password (no lower case alphabetical character)</t>
-  </si>
-  <si>
-    <t>negative case - wrong password (no upper case alphabetical character)</t>
-  </si>
-  <si>
-    <t>negative case - wrong password (no numerical character)</t>
-  </si>
-  <si>
-    <t>negative case - wrong password (below 8 characters)</t>
-  </si>
-  <si>
-    <t>negative case - wrong password (exceed 16 characters)</t>
-  </si>
-  <si>
     <t>+6281234567890</t>
   </si>
   <si>
@@ -202,93 +163,6 @@
     <t>PasswordMelebihi16Karakter</t>
   </si>
   <si>
-    <t>negative case - wrong full name, email, phone number, password, confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, email, phone number, password</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, email, phone number</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, email, password, confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, email, phone number, confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, email, password</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, email</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, phone number, password, confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong email, phone number, password, confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong phone number, password, confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong password, confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong email, password, confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, password, confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, email, confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, phone number , confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, phone number, password</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, phone number</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, password</t>
-  </si>
-  <si>
-    <t>negative case - wrong email, phone number, password</t>
-  </si>
-  <si>
-    <t>negative case - wrong email, password</t>
-  </si>
-  <si>
-    <t>negative case - wrong phone number, password</t>
-  </si>
-  <si>
-    <t>negative case - wrong email</t>
-  </si>
-  <si>
-    <t>negative case - wrong email, confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name, confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name</t>
-  </si>
-  <si>
-    <t>negative case - wrong email, phone number, confirm password</t>
-  </si>
-  <si>
-    <t>negative case - wrong email, phone number</t>
-  </si>
-  <si>
-    <t>negative case - wrong phone number, confirm password</t>
-  </si>
-  <si>
     <t>positive case - correct full name, email, phone number, password, confirm password</t>
   </si>
   <si>
@@ -328,36 +202,6 @@
     <t>negative case - invalid token</t>
   </si>
   <si>
-    <t>negative case - wrong full name (below 3 characters)</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name (non alphabetical)</t>
-  </si>
-  <si>
-    <t>negative case - wrong full name (exceed 20 characters)</t>
-  </si>
-  <si>
-    <t>negative case - wrong email (no @)</t>
-  </si>
-  <si>
-    <t>negative case - wrong confirm password (no lower case alphabetical character)</t>
-  </si>
-  <si>
-    <t>negative case - wrong confirm password (no upper case alphabetical character)</t>
-  </si>
-  <si>
-    <t>negative case - wrong confirm password (no numerical character)</t>
-  </si>
-  <si>
-    <t>negative case - wrong confirm password (below 8 characters)</t>
-  </si>
-  <si>
-    <t>negative case - wrong confirm password (exceed 16 characters)</t>
-  </si>
-  <si>
-    <t>negative case - wrong new password and email</t>
-  </si>
-  <si>
     <t>positif case - correct new password and email</t>
   </si>
   <si>
@@ -365,6 +209,165 @@
   </si>
   <si>
     <t>+601300808888</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, email, phone number, password, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, email, phone number, password</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, email, phone number, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, email, phone number</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, email, password, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, email, password</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, email, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, email</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, phone number, password, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, phone number, password</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, phone number , confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, phone number</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, password, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, password</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name</t>
+  </si>
+  <si>
+    <t>negative case - invalid email, phone number, password, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid email, phone number, password</t>
+  </si>
+  <si>
+    <t>negative case - invalid email, phone number, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid email, phone number</t>
+  </si>
+  <si>
+    <t>negative case - invalid email, password, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid email, password</t>
+  </si>
+  <si>
+    <t>negative case - invalid email, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid email</t>
+  </si>
+  <si>
+    <t>negative case - inalid phone number, password, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number, password</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number</t>
+  </si>
+  <si>
+    <t>negative case - invalid password, confirm password</t>
+  </si>
+  <si>
+    <t>negative case - inavalid password</t>
+  </si>
+  <si>
+    <t>negative case - invalid confirm password</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name (below 3 characters)</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name (exceed 20 characters)</t>
+  </si>
+  <si>
+    <t>negative case - invalid full name (non alphabetical)</t>
+  </si>
+  <si>
+    <t>negative case - invalid email (no @)</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number format (not numerical)</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number format (exceed 12 characters)</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number (outside Indonesia)</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number (unregistered number)</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number (unverified number)</t>
+  </si>
+  <si>
+    <t>negative case - invalid password (no lower case alphabetical character)</t>
+  </si>
+  <si>
+    <t>negative case - invalid password (no upper case alphabetical character)</t>
+  </si>
+  <si>
+    <t>negative case - invalid password (no numerical character)</t>
+  </si>
+  <si>
+    <t>negative case - invalid password (below 8 characters)</t>
+  </si>
+  <si>
+    <t>negative case - invalid password (exceed 16 characters)</t>
+  </si>
+  <si>
+    <t>negative case - invalid confirm password (no lower case alphabetical character)</t>
+  </si>
+  <si>
+    <t>negative case - invalid confirm password (no upper case alphabetical character)</t>
+  </si>
+  <si>
+    <t>negative case - invalid confirm password (no numerical character)</t>
+  </si>
+  <si>
+    <t>negative case - invalid confirm password (below 8 characters)</t>
+  </si>
+  <si>
+    <t>negative case - invalid confirm password (exceed 16 characters)</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number and password</t>
+  </si>
+  <si>
+    <t>negative case - invalid password</t>
+  </si>
+  <si>
+    <t>negative case - invalid new password and email</t>
   </si>
 </sst>
 </file>
@@ -857,7 +860,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -901,7 +904,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>28</v>
@@ -925,13 +928,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>17</v>
@@ -949,7 +952,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>4</v>
@@ -979,7 +982,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>7</v>
@@ -995,13 +998,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>17</v>
@@ -1019,13 +1022,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="B7" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>36</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>49</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>17</v>
@@ -1043,13 +1046,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>17</v>
@@ -1067,13 +1070,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>17</v>
@@ -1091,13 +1094,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>17</v>
@@ -1115,13 +1118,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>17</v>
@@ -1139,13 +1142,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>17</v>
@@ -1163,13 +1166,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>17</v>
@@ -1187,13 +1190,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>17</v>
@@ -1211,13 +1214,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>17</v>
@@ -1341,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7189700-26BE-B342-926E-EF81568121D9}">
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1410,7 +1413,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1444,7 +1447,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -1478,7 +1481,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
@@ -1512,7 +1515,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
@@ -1546,7 +1549,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
@@ -1580,7 +1583,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -1614,7 +1617,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -1648,7 +1651,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -1682,7 +1685,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="24"/>
@@ -1716,7 +1719,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="24"/>
@@ -1750,7 +1753,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" s="26"/>
       <c r="C12" s="24"/>
@@ -1784,7 +1787,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="24"/>
@@ -1818,7 +1821,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="24"/>
@@ -1852,7 +1855,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="24"/>
@@ -1886,7 +1889,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="24"/>
@@ -1920,7 +1923,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="24"/>
@@ -1954,7 +1957,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="26"/>
@@ -1988,7 +1991,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="26"/>
@@ -2022,7 +2025,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="26"/>
@@ -2056,7 +2059,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="26"/>
@@ -2090,7 +2093,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="26"/>
@@ -2124,7 +2127,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B23" s="24"/>
       <c r="C23" s="26"/>
@@ -2158,7 +2161,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B24" s="24"/>
       <c r="C24" s="26"/>
@@ -2192,7 +2195,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B25" s="24"/>
       <c r="C25" s="26"/>
@@ -2226,7 +2229,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B26" s="24"/>
       <c r="C26" s="24"/>
@@ -2260,7 +2263,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
@@ -2294,7 +2297,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="24"/>
@@ -2328,7 +2331,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="B29" s="24"/>
       <c r="C29" s="24"/>
@@ -2362,7 +2365,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="B30" s="24"/>
       <c r="C30" s="24"/>
@@ -2396,7 +2399,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="B31" s="24"/>
       <c r="C31" s="24"/>
@@ -2430,7 +2433,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="B32" s="24"/>
       <c r="C32" s="24"/>
@@ -2464,7 +2467,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
@@ -2494,7 +2497,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="B34" s="28"/>
       <c r="C34" s="31"/>
@@ -2509,7 +2512,7 @@
         <v>21</v>
       </c>
       <c r="J34" s="29" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="K34" s="29" t="s">
         <v>6</v>
@@ -2526,7 +2529,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="B35" s="28"/>
       <c r="C35" s="31"/>
@@ -2541,7 +2544,7 @@
         <v>21</v>
       </c>
       <c r="J35" s="29" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="K35" s="28" t="s">
         <v>5</v>
@@ -2558,7 +2561,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="B36" s="28"/>
       <c r="C36" s="31"/>
@@ -2573,7 +2576,7 @@
         <v>21</v>
       </c>
       <c r="J36" s="29" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="K36" s="29" t="s">
         <v>6</v>
@@ -2590,7 +2593,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="B37" s="28"/>
       <c r="C37" s="31"/>
@@ -2605,7 +2608,7 @@
         <v>21</v>
       </c>
       <c r="J37" s="29" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="K37" s="28" t="s">
         <v>5</v>
@@ -2622,7 +2625,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="B38" s="28"/>
       <c r="C38" s="31"/>
@@ -2637,7 +2640,7 @@
         <v>21</v>
       </c>
       <c r="J38" s="29" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="K38" s="29" t="s">
         <v>6</v>
@@ -2654,7 +2657,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="B39" s="28"/>
       <c r="C39" s="31"/>
@@ -2669,7 +2672,7 @@
         <v>21</v>
       </c>
       <c r="J39" s="29" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="K39" s="28" t="s">
         <v>5</v>
@@ -2686,7 +2689,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="B40" s="28"/>
       <c r="C40" s="31"/>
@@ -2701,7 +2704,7 @@
         <v>21</v>
       </c>
       <c r="J40" s="29" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="K40" s="29" t="s">
         <v>6</v>
@@ -2718,7 +2721,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="B41" s="28"/>
       <c r="C41" s="31"/>
@@ -2748,7 +2751,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="B42" s="28"/>
       <c r="C42" s="31"/>
@@ -2778,7 +2781,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="B43" s="28"/>
       <c r="C43" s="31"/>
@@ -2808,7 +2811,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B44" s="18"/>
       <c r="C44" s="23"/>
@@ -2842,7 +2845,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B45" s="18"/>
       <c r="C45" s="23"/>
@@ -2876,7 +2879,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B46" s="18"/>
       <c r="C46" s="23"/>
@@ -2910,7 +2913,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B47" s="23"/>
       <c r="C47" s="18"/>
@@ -2944,7 +2947,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="B48" s="23"/>
       <c r="C48" s="23"/>
@@ -2978,7 +2981,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="B49" s="23"/>
       <c r="C49" s="23"/>
@@ -3012,7 +3015,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="B50" s="23"/>
       <c r="C50" s="23"/>
@@ -3046,7 +3049,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="B51" s="23"/>
       <c r="C51" s="23"/>
@@ -3080,7 +3083,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="B52" s="23"/>
       <c r="C52" s="23"/>
@@ -3114,7 +3117,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="B53" s="23"/>
       <c r="C53" s="23"/>
@@ -3148,7 +3151,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="22" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="B54" s="23"/>
       <c r="C54" s="23"/>
@@ -3182,7 +3185,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="22" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="B55" s="23"/>
       <c r="C55" s="23"/>
@@ -3216,7 +3219,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="22" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="B56" s="23"/>
       <c r="C56" s="23"/>
@@ -3250,7 +3253,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="22" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="B57" s="23"/>
       <c r="C57" s="23"/>
@@ -3284,7 +3287,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="22" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B58" s="23"/>
       <c r="C58" s="23"/>
@@ -3318,7 +3321,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B59" s="23"/>
       <c r="C59" s="23"/>
@@ -3352,7 +3355,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B60" s="23"/>
       <c r="C60" s="23"/>
@@ -3386,7 +3389,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B61" s="23"/>
       <c r="C61" s="23"/>
@@ -3420,7 +3423,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B62" s="23"/>
       <c r="C62" s="23"/>
@@ -3463,7 +3466,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3519,7 +3522,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -3546,7 +3549,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="31"/>
@@ -3573,7 +3576,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="30"/>
@@ -3600,7 +3603,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5" s="31"/>
@@ -3625,7 +3628,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="31"/>
@@ -3652,7 +3655,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="28"/>
@@ -3679,7 +3682,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="28"/>
@@ -3706,7 +3709,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="28"/>
@@ -3733,7 +3736,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="31"/>
@@ -3760,7 +3763,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B11" s="31"/>
       <c r="C11" s="29"/>
@@ -3787,7 +3790,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="B12" s="28"/>
       <c r="C12" s="28"/>
@@ -3812,7 +3815,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="B13" s="31"/>
       <c r="C13" s="31"/>
@@ -3837,7 +3840,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>

</xml_diff>

<commit_message>
eight commit - add delete feature for register automation testing
</commit_message>
<xml_diff>
--- a/resources/DataLoginMenu.xlsx
+++ b/resources/DataLoginMenu.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/G2Lab/FinalProject/QuotaAppTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA75AC57-3580-A946-97EB-989600C1707C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2736A7-D42F-1E4E-9A0E-DD62451DF5C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Register" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
-    <sheet name="Forgot Password" sheetId="3" r:id="rId4"/>
+    <sheet name="Forgot Password" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="170">
   <si>
     <t>password</t>
   </si>
@@ -128,9 +127,6 @@
     <t>wrong password</t>
   </si>
   <si>
-    <t>+628123456789101112</t>
-  </si>
-  <si>
     <t>+6281234567890</t>
   </si>
   <si>
@@ -215,9 +211,6 @@
     <t>negative case - invalid phone number format (not numerical)</t>
   </si>
   <si>
-    <t>negative case - invalid phone number format (exceed 12 characters)</t>
-  </si>
-  <si>
     <t>negative case - invalid phone number (outside Indonesia)</t>
   </si>
   <si>
@@ -543,6 +536,15 @@
   </si>
   <si>
     <t>positive case - valid phone number and password</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number format (exceed 15 characters)</t>
+  </si>
+  <si>
+    <t>+628123456789101112222</t>
+  </si>
+  <si>
+    <t>size must be between 0 and 20</t>
   </si>
 </sst>
 </file>
@@ -1006,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9959BB-4BD4-1645-834F-8040D5B979C6}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1038,7 +1040,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>26</v>
@@ -1055,13 +1057,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>24</v>
@@ -1072,7 +1074,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>4</v>
@@ -1089,13 +1091,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>7</v>
@@ -1106,13 +1108,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>24</v>
@@ -1123,13 +1125,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>59</v>
+        <v>167</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>24</v>
@@ -1140,13 +1142,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>24</v>
@@ -1157,13 +1159,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>24</v>
@@ -1174,13 +1176,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>24</v>
@@ -1191,13 +1193,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>15</v>
@@ -1208,13 +1210,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>15</v>
@@ -1225,13 +1227,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>15</v>
@@ -1242,13 +1244,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>15</v>
@@ -1259,13 +1261,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>15</v>
@@ -1276,13 +1278,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>15</v>
@@ -1301,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7189700-26BE-B342-926E-EF81568121D9}">
   <dimension ref="A1:O99"/>
   <sheetViews>
-    <sheetView topLeftCell="E43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" topLeftCell="G8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1311,10 +1313,10 @@
     <col min="2" max="2" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="25.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
@@ -1329,7 +1331,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>8</v>
@@ -1373,31 +1375,31 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>22</v>
@@ -1420,31 +1422,31 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>24</v>
+        <v>169</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>22</v>
@@ -1467,31 +1469,31 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>22</v>
@@ -1514,31 +1516,31 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>22</v>
@@ -1561,31 +1563,31 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>33</v>
-      </c>
       <c r="G6" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>24</v>
+        <v>169</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>22</v>
@@ -1608,31 +1610,31 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>22</v>
@@ -1655,31 +1657,31 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>22</v>
@@ -1702,25 +1704,25 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>24</v>
@@ -1749,25 +1751,25 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>24</v>
@@ -1796,25 +1798,25 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>24</v>
@@ -1843,25 +1845,25 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>24</v>
@@ -1890,25 +1892,25 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>24</v>
@@ -1937,25 +1939,25 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>24</v>
@@ -1984,25 +1986,25 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>24</v>
@@ -2031,25 +2033,25 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>24</v>
@@ -2078,25 +2080,25 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>24</v>
@@ -2125,31 +2127,31 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>22</v>
@@ -2172,31 +2174,31 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>22</v>
@@ -2219,31 +2221,31 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>22</v>
@@ -2266,31 +2268,31 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>22</v>
@@ -2313,31 +2315,31 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>22</v>
@@ -2360,31 +2362,31 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>22</v>
@@ -2407,31 +2409,31 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>22</v>
@@ -2454,31 +2456,31 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>22</v>
@@ -2501,31 +2503,31 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>22</v>
@@ -2548,31 +2550,31 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>22</v>
@@ -2595,31 +2597,31 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>22</v>
@@ -2642,25 +2644,25 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>24</v>
@@ -2689,25 +2691,25 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>24</v>
@@ -2736,25 +2738,25 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>24</v>
@@ -2783,25 +2785,25 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>24</v>
@@ -2830,25 +2832,25 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>24</v>
@@ -2877,31 +2879,31 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>22</v>
@@ -2924,31 +2926,31 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>24</v>
+        <v>169</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>22</v>
@@ -2971,31 +2973,31 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>22</v>
@@ -3018,31 +3020,31 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>22</v>
@@ -3065,31 +3067,31 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E38" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F38" s="10" t="s">
-        <v>33</v>
-      </c>
       <c r="G38" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>22</v>
@@ -3112,31 +3114,31 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>22</v>
@@ -3159,31 +3161,31 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>22</v>
@@ -3206,31 +3208,31 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>22</v>
@@ -3253,31 +3255,31 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E42" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>22</v>
@@ -3300,31 +3302,31 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>22</v>
@@ -3347,31 +3349,31 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>22</v>
@@ -3394,31 +3396,31 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E45" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>22</v>
@@ -3441,31 +3443,31 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>22</v>
@@ -3488,31 +3490,31 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>22</v>
@@ -3535,31 +3537,31 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>22</v>
@@ -3582,31 +3584,31 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>22</v>
@@ -3629,31 +3631,31 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>22</v>
@@ -3676,31 +3678,31 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>22</v>
@@ -3723,31 +3725,31 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>22</v>
@@ -3770,31 +3772,31 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>22</v>
@@ -3817,31 +3819,31 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>22</v>
@@ -3864,31 +3866,31 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>22</v>
@@ -3911,31 +3913,31 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>22</v>
@@ -3958,31 +3960,31 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>22</v>
@@ -4005,31 +4007,31 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>22</v>
@@ -4052,31 +4054,31 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>22</v>
@@ -4099,31 +4101,31 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>22</v>
@@ -4146,31 +4148,31 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E61" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>22</v>
@@ -4193,31 +4195,31 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>22</v>
@@ -4240,31 +4242,31 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H63" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>22</v>
@@ -4287,31 +4289,31 @@
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>22</v>
@@ -4334,25 +4336,25 @@
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H65" s="16" t="s">
         <v>7</v>
@@ -4376,36 +4378,36 @@
         <v>7</v>
       </c>
       <c r="O65" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H66" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>22</v>
@@ -4428,31 +4430,31 @@
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H67" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J67" s="4" t="s">
         <v>22</v>
@@ -4475,31 +4477,31 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H68" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>22</v>
@@ -4522,25 +4524,25 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F69" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>24</v>
@@ -4569,31 +4571,31 @@
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>22</v>
@@ -4616,31 +4618,31 @@
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>22</v>
@@ -4663,31 +4665,31 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H72" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>22</v>
@@ -4710,31 +4712,31 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E73" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H73" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>22</v>
@@ -4757,31 +4759,31 @@
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>59</v>
+        <v>167</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>22</v>
@@ -4804,31 +4806,31 @@
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G75" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H75" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>22</v>
@@ -4851,31 +4853,31 @@
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H76" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J76" s="4" t="s">
         <v>22</v>
@@ -4898,31 +4900,31 @@
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H77" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>22</v>
@@ -4945,31 +4947,31 @@
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F78" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H78" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J78" s="4" t="s">
         <v>22</v>
@@ -4992,31 +4994,31 @@
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H79" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>22</v>
@@ -5039,31 +5041,31 @@
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J80" s="4" t="s">
         <v>22</v>
@@ -5086,31 +5088,31 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H81" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J81" s="4" t="s">
         <v>22</v>
@@ -5133,31 +5135,31 @@
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F82" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H82" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J82" s="4" t="s">
         <v>22</v>
@@ -5180,31 +5182,31 @@
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H83" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J83" s="4" t="s">
         <v>22</v>
@@ -5227,31 +5229,31 @@
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H84" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J84" s="4" t="s">
         <v>22</v>
@@ -5274,31 +5276,31 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H85" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J85" s="4" t="s">
         <v>22</v>
@@ -5321,31 +5323,31 @@
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H86" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J86" s="4" t="s">
         <v>22</v>
@@ -5368,31 +5370,31 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D87" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H87" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J87" s="4" t="s">
         <v>22</v>
@@ -5415,31 +5417,31 @@
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F88" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H88" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J88" s="4" t="s">
         <v>22</v>
@@ -5462,31 +5464,31 @@
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F89" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G89" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H89" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J89" s="4" t="s">
         <v>22</v>
@@ -5509,25 +5511,25 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>7</v>
@@ -5539,7 +5541,7 @@
         <v>19</v>
       </c>
       <c r="K90" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L90" s="17" t="s">
         <v>6</v>
@@ -5548,7 +5550,7 @@
         <v>22</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O90" s="6" t="s">
         <v>25</v>
@@ -5556,25 +5558,25 @@
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>7</v>
@@ -5586,7 +5588,7 @@
         <v>19</v>
       </c>
       <c r="K91" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L91" s="16" t="s">
         <v>5</v>
@@ -5595,7 +5597,7 @@
         <v>22</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O91" s="6" t="s">
         <v>25</v>
@@ -5603,25 +5605,25 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F92" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>7</v>
@@ -5633,7 +5635,7 @@
         <v>19</v>
       </c>
       <c r="K92" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L92" s="17" t="s">
         <v>6</v>
@@ -5642,7 +5644,7 @@
         <v>22</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O92" s="6" t="s">
         <v>25</v>
@@ -5650,25 +5652,25 @@
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F93" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>7</v>
@@ -5680,7 +5682,7 @@
         <v>19</v>
       </c>
       <c r="K93" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L93" s="16" t="s">
         <v>5</v>
@@ -5689,7 +5691,7 @@
         <v>22</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O93" s="6" t="s">
         <v>25</v>
@@ -5697,25 +5699,25 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F94" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>7</v>
@@ -5727,7 +5729,7 @@
         <v>19</v>
       </c>
       <c r="K94" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L94" s="17" t="s">
         <v>6</v>
@@ -5736,7 +5738,7 @@
         <v>22</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O94" s="6" t="s">
         <v>25</v>
@@ -5744,25 +5746,25 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E95" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G95" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>7</v>
@@ -5774,7 +5776,7 @@
         <v>19</v>
       </c>
       <c r="K95" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L95" s="16" t="s">
         <v>5</v>
@@ -5783,7 +5785,7 @@
         <v>22</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O95" s="6" t="s">
         <v>25</v>
@@ -5791,25 +5793,25 @@
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F96" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G96" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>7</v>
@@ -5821,7 +5823,7 @@
         <v>19</v>
       </c>
       <c r="K96" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L96" s="17" t="s">
         <v>6</v>
@@ -5830,7 +5832,7 @@
         <v>22</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O96" s="6" t="s">
         <v>25</v>
@@ -5838,25 +5840,25 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D97" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E97" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F97" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>7</v>
@@ -5874,10 +5876,10 @@
         <v>22</v>
       </c>
       <c r="M97" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O97" s="6" t="s">
         <v>25</v>
@@ -5885,25 +5887,25 @@
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E98" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F98" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G98" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>7</v>
@@ -5921,10 +5923,10 @@
         <v>22</v>
       </c>
       <c r="M98" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O98" s="6" t="s">
         <v>25</v>
@@ -5932,25 +5934,25 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D99" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F99" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G99" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>7</v>
@@ -5968,10 +5970,10 @@
         <v>22</v>
       </c>
       <c r="M99" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O99" s="6" t="s">
         <v>25</v>
@@ -5995,31 +5997,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053ABF5C-1DC4-A042-A68F-E691DE0937C1}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O31" sqref="A1:O31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24BE3DA-8EEA-0F42-A704-7573A8A4E5B9}">
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="60.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
@@ -6069,19 +6057,19 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>22</v>
@@ -6104,13 +6092,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>24</v>
@@ -6139,19 +6127,19 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>22</v>
@@ -6174,13 +6162,13 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>7</v>
@@ -6209,13 +6197,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>24</v>
@@ -6244,13 +6232,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>59</v>
+        <v>167</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>24</v>
@@ -6279,13 +6267,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>24</v>
@@ -6314,13 +6302,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>24</v>
@@ -6349,13 +6337,13 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>24</v>
@@ -6384,19 +6372,19 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>22</v>
@@ -6419,13 +6407,13 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>7</v>
@@ -6454,13 +6442,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>7</v>
@@ -6489,13 +6477,13 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
test all test cases
</commit_message>
<xml_diff>
--- a/resources/DataLoginMenu.xlsx
+++ b/resources/DataLoginMenu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/G2Lab/FinalProject/QuotaAppTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6495BBBA-0E0A-094D-9C17-4354FD680BE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5864B591-92BB-CB46-B17B-12531E551622}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -511,12 +511,6 @@
     <t>Your pin length transaksi must be 6</t>
   </si>
   <si>
-    <t>Length nama user must be more than equals 3 character</t>
-  </si>
-  <si>
-    <t>Your phone number must be less than equals 15</t>
-  </si>
-  <si>
     <t>Your password must contains one lowercase characters</t>
   </si>
   <si>
@@ -653,6 +647,12 @@
   </si>
   <si>
     <t>testforgotpasswordbackend@gmail.com</t>
+  </si>
+  <si>
+    <t>Length nama user must be less than 3 character</t>
+  </si>
+  <si>
+    <t>Your phone number must be less than 15</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1161,7 @@
         <v>23</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1178,7 +1178,7 @@
         <v>23</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1229,7 +1229,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1246,7 +1246,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1263,7 +1263,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1280,7 +1280,7 @@
         <v>23</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1297,7 +1297,7 @@
         <v>23</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1412,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7189700-26BE-B342-926E-EF81568121D9}">
   <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1477,7 +1477,7 @@
         <v>3</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>16</v>
@@ -1494,7 +1494,7 @@
         <v>147</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>25</v>
@@ -1541,7 +1541,7 @@
         <v>147</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>25</v>
@@ -1588,7 +1588,7 @@
         <v>147</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>25</v>
@@ -1635,7 +1635,7 @@
         <v>147</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>25</v>
@@ -1682,7 +1682,7 @@
         <v>147</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>4</v>
@@ -1729,7 +1729,7 @@
         <v>147</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>4</v>
@@ -1776,7 +1776,7 @@
         <v>147</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>4</v>
@@ -1823,7 +1823,7 @@
         <v>147</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>4</v>
@@ -1870,7 +1870,7 @@
         <v>147</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>25</v>
@@ -1917,7 +1917,7 @@
         <v>147</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>25</v>
@@ -1964,7 +1964,7 @@
         <v>147</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>25</v>
@@ -2011,7 +2011,7 @@
         <v>147</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>25</v>
@@ -2058,7 +2058,7 @@
         <v>147</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>4</v>
@@ -2105,7 +2105,7 @@
         <v>147</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>4</v>
@@ -2152,7 +2152,7 @@
         <v>147</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>4</v>
@@ -2199,7 +2199,7 @@
         <v>147</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>4</v>
@@ -2246,7 +2246,7 @@
         <v>64</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>25</v>
@@ -2293,7 +2293,7 @@
         <v>64</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>25</v>
@@ -2340,7 +2340,7 @@
         <v>64</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>25</v>
@@ -2387,7 +2387,7 @@
         <v>64</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E21" s="16" t="s">
         <v>25</v>
@@ -2434,7 +2434,7 @@
         <v>64</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>4</v>
@@ -2481,7 +2481,7 @@
         <v>64</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>4</v>
@@ -2528,7 +2528,7 @@
         <v>64</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>4</v>
@@ -2575,7 +2575,7 @@
         <v>64</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>4</v>
@@ -2622,7 +2622,7 @@
         <v>64</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E26" s="16" t="s">
         <v>25</v>
@@ -2669,7 +2669,7 @@
         <v>64</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>25</v>
@@ -2716,7 +2716,7 @@
         <v>64</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E28" s="16" t="s">
         <v>25</v>
@@ -2763,7 +2763,7 @@
         <v>64</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E29" s="16" t="s">
         <v>25</v>
@@ -2810,7 +2810,7 @@
         <v>64</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>4</v>
@@ -2857,7 +2857,7 @@
         <v>64</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>4</v>
@@ -2904,7 +2904,7 @@
         <v>64</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>4</v>
@@ -2951,7 +2951,7 @@
         <v>64</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>4</v>
@@ -2998,7 +2998,7 @@
         <v>147</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E34" s="16" t="s">
         <v>25</v>
@@ -3045,7 +3045,7 @@
         <v>147</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>25</v>
@@ -3092,7 +3092,7 @@
         <v>147</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E36" s="16" t="s">
         <v>25</v>
@@ -3139,7 +3139,7 @@
         <v>147</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E37" s="16" t="s">
         <v>25</v>
@@ -3186,7 +3186,7 @@
         <v>147</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>4</v>
@@ -3233,7 +3233,7 @@
         <v>147</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>4</v>
@@ -3280,7 +3280,7 @@
         <v>147</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>4</v>
@@ -3327,7 +3327,7 @@
         <v>147</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>4</v>
@@ -3374,7 +3374,7 @@
         <v>147</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E42" s="16" t="s">
         <v>25</v>
@@ -3421,7 +3421,7 @@
         <v>147</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>25</v>
@@ -3468,7 +3468,7 @@
         <v>147</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E44" s="16" t="s">
         <v>25</v>
@@ -3515,7 +3515,7 @@
         <v>147</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E45" s="16" t="s">
         <v>25</v>
@@ -3562,7 +3562,7 @@
         <v>147</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>4</v>
@@ -3609,7 +3609,7 @@
         <v>147</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>4</v>
@@ -3656,7 +3656,7 @@
         <v>147</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>4</v>
@@ -3703,7 +3703,7 @@
         <v>147</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>4</v>
@@ -3750,7 +3750,7 @@
         <v>64</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E50" s="16" t="s">
         <v>25</v>
@@ -3797,7 +3797,7 @@
         <v>64</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E51" s="16" t="s">
         <v>25</v>
@@ -3844,7 +3844,7 @@
         <v>64</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>25</v>
@@ -3891,7 +3891,7 @@
         <v>64</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>25</v>
@@ -3938,7 +3938,7 @@
         <v>64</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>4</v>
@@ -3985,7 +3985,7 @@
         <v>64</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>4</v>
@@ -4032,7 +4032,7 @@
         <v>64</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>4</v>
@@ -4079,7 +4079,7 @@
         <v>64</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>4</v>
@@ -4126,7 +4126,7 @@
         <v>64</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>25</v>
@@ -4173,7 +4173,7 @@
         <v>64</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>25</v>
@@ -4220,7 +4220,7 @@
         <v>64</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>25</v>
@@ -4267,7 +4267,7 @@
         <v>64</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>25</v>
@@ -4314,7 +4314,7 @@
         <v>64</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>4</v>
@@ -4361,7 +4361,7 @@
         <v>64</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>4</v>
@@ -4408,7 +4408,7 @@
         <v>64</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>4</v>
@@ -4455,7 +4455,7 @@
         <v>64</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>4</v>
@@ -4502,7 +4502,7 @@
         <v>64</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>4</v>
@@ -4549,7 +4549,7 @@
         <v>64</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>4</v>
@@ -4596,7 +4596,7 @@
         <v>64</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>4</v>
@@ -4643,7 +4643,7 @@
         <v>58</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>4</v>
@@ -4658,7 +4658,7 @@
         <v>23</v>
       </c>
       <c r="I69" s="16" t="s">
-        <v>158</v>
+        <v>204</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>21</v>
@@ -4690,7 +4690,7 @@
         <v>59</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>4</v>
@@ -4737,7 +4737,7 @@
         <v>60</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>4</v>
@@ -4784,7 +4784,7 @@
         <v>64</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>4</v>
@@ -4831,7 +4831,7 @@
         <v>64</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E73" s="16" t="s">
         <v>25</v>
@@ -4878,7 +4878,7 @@
         <v>64</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E74" s="17" t="s">
         <v>145</v>
@@ -4893,7 +4893,7 @@
         <v>23</v>
       </c>
       <c r="I74" s="16" t="s">
-        <v>159</v>
+        <v>205</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>21</v>
@@ -4925,7 +4925,7 @@
         <v>64</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E75" s="17" t="s">
         <v>35</v>
@@ -4963,7 +4963,7 @@
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B76" s="10" t="s">
         <v>77</v>
@@ -4972,7 +4972,7 @@
         <v>64</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E76" s="17" t="s">
         <v>27</v>
@@ -5019,7 +5019,7 @@
         <v>64</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E77" s="17" t="s">
         <v>28</v>
@@ -5066,7 +5066,7 @@
         <v>64</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>4</v>
@@ -5081,7 +5081,7 @@
         <v>23</v>
       </c>
       <c r="I78" s="16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J78" s="4" t="s">
         <v>21</v>
@@ -5113,7 +5113,7 @@
         <v>64</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>4</v>
@@ -5128,7 +5128,7 @@
         <v>23</v>
       </c>
       <c r="I79" s="16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>21</v>
@@ -5160,7 +5160,7 @@
         <v>64</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>4</v>
@@ -5207,7 +5207,7 @@
         <v>64</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>4</v>
@@ -5254,7 +5254,7 @@
         <v>64</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>4</v>
@@ -5301,7 +5301,7 @@
         <v>64</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>4</v>
@@ -5348,7 +5348,7 @@
         <v>64</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>4</v>
@@ -5395,7 +5395,7 @@
         <v>64</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>4</v>
@@ -5442,7 +5442,7 @@
         <v>64</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>4</v>
@@ -5489,7 +5489,7 @@
         <v>64</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>4</v>
@@ -5536,7 +5536,7 @@
         <v>64</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>4</v>
@@ -5583,7 +5583,7 @@
         <v>64</v>
       </c>
       <c r="D89" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>4</v>
@@ -5621,7 +5621,7 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B90" s="10" t="s">
         <v>77</v>
@@ -5630,7 +5630,7 @@
         <v>64</v>
       </c>
       <c r="D90" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>4</v>
@@ -5651,7 +5651,7 @@
         <v>18</v>
       </c>
       <c r="K90" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L90" s="18" t="s">
         <v>6</v>
@@ -5677,7 +5677,7 @@
         <v>64</v>
       </c>
       <c r="D91" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>4</v>
@@ -5698,7 +5698,7 @@
         <v>18</v>
       </c>
       <c r="K91" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L91" s="12" t="s">
         <v>5</v>
@@ -5715,7 +5715,7 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B92" s="10" t="s">
         <v>77</v>
@@ -5724,7 +5724,7 @@
         <v>64</v>
       </c>
       <c r="D92" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>4</v>
@@ -5762,7 +5762,7 @@
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B93" s="10" t="s">
         <v>77</v>
@@ -5771,7 +5771,7 @@
         <v>64</v>
       </c>
       <c r="D93" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>4</v>
@@ -5809,7 +5809,7 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B94" s="10" t="s">
         <v>77</v>
@@ -5818,7 +5818,7 @@
         <v>64</v>
       </c>
       <c r="D94" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>4</v>
@@ -5839,7 +5839,7 @@
         <v>18</v>
       </c>
       <c r="K94" s="18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="L94" s="12" t="s">
         <v>5</v>
@@ -5856,7 +5856,7 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B95" s="10" t="s">
         <v>77</v>
@@ -5865,7 +5865,7 @@
         <v>64</v>
       </c>
       <c r="D95" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>4</v>
@@ -5886,13 +5886,13 @@
         <v>18</v>
       </c>
       <c r="K95" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="L95" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M95" s="16" t="s">
-        <v>186</v>
+        <v>182</v>
+      </c>
+      <c r="L95" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M95" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="N95" s="18" t="s">
         <v>149</v>
@@ -5903,7 +5903,7 @@
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>77</v>
@@ -5912,7 +5912,7 @@
         <v>64</v>
       </c>
       <c r="D96" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>4</v>
@@ -5933,7 +5933,7 @@
         <v>18</v>
       </c>
       <c r="K96" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L96" s="12" t="s">
         <v>5</v>
@@ -5950,7 +5950,7 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B97" s="10" t="s">
         <v>77</v>
@@ -5959,7 +5959,7 @@
         <v>64</v>
       </c>
       <c r="D97" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>4</v>
@@ -6006,7 +6006,7 @@
         <v>64</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>4</v>
@@ -6027,7 +6027,7 @@
         <v>18</v>
       </c>
       <c r="K98" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L98" s="12" t="s">
         <v>5</v>
@@ -6044,7 +6044,7 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B99" s="10" t="s">
         <v>77</v>
@@ -6053,7 +6053,7 @@
         <v>64</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>4</v>
@@ -6100,7 +6100,7 @@
         <v>64</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>4</v>
@@ -6127,10 +6127,10 @@
         <v>21</v>
       </c>
       <c r="M100" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N100" s="18" t="s">
-        <v>23</v>
+        <v>149</v>
       </c>
       <c r="O100" s="19" t="s">
         <v>24</v>
@@ -6152,8 +6152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24BE3DA-8EEA-0F42-A704-7573A8A4E5B9}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:A39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6204,22 +6204,22 @@
         <v>3</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>16</v>
       </c>
       <c r="L1" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="M1" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -6230,7 +6230,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>23</v>
@@ -6277,13 +6277,13 @@
         <v>25</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>21</v>
@@ -6324,7 +6324,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>23</v>
@@ -6365,13 +6365,13 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>7</v>
@@ -6395,7 +6395,7 @@
         <v>7</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>62</v>
@@ -6418,13 +6418,13 @@
         <v>25</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>21</v>
@@ -6465,13 +6465,13 @@
         <v>145</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>21</v>
@@ -6512,13 +6512,13 @@
         <v>35</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>21</v>
@@ -6559,13 +6559,13 @@
         <v>27</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>21</v>
@@ -6606,13 +6606,13 @@
         <v>28</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>21</v>
@@ -6653,7 +6653,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>23</v>
@@ -6694,13 +6694,13 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>7</v>
@@ -6712,7 +6712,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>6</v>
@@ -6747,7 +6747,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>7</v>
@@ -6759,7 +6759,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>5</v>
@@ -6788,13 +6788,13 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>7</v>
@@ -6835,13 +6835,13 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>7</v>
@@ -6865,7 +6865,7 @@
         <v>7</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L15" s="12" t="s">
         <v>62</v>
@@ -6882,13 +6882,13 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>7</v>
@@ -6900,7 +6900,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>5</v>
@@ -6929,13 +6929,13 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>7</v>
@@ -6947,7 +6947,7 @@
         <v>18</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H17" s="10" t="s">
         <v>5</v>
@@ -6976,13 +6976,13 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>7</v>
@@ -6994,7 +6994,7 @@
         <v>18</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>5</v>
@@ -7023,13 +7023,13 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>7</v>
@@ -7076,7 +7076,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>7</v>
@@ -7088,7 +7088,7 @@
         <v>18</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H20" s="10" t="s">
         <v>5</v>
@@ -7117,13 +7117,13 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>7</v>
@@ -7147,7 +7147,7 @@
         <v>7</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L21" s="12" t="s">
         <v>62</v>
@@ -7170,7 +7170,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>7</v>
@@ -7188,7 +7188,7 @@
         <v>21</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J22" s="18" t="s">
         <v>149</v>
@@ -7211,13 +7211,13 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>7</v>
@@ -7241,7 +7241,7 @@
         <v>7</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L23" s="18" t="s">
         <v>69</v>
@@ -7258,13 +7258,13 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>7</v>
@@ -7288,7 +7288,7 @@
         <v>7</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L24" s="18" t="s">
         <v>69</v>
@@ -7305,13 +7305,13 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>7</v>
@@ -7335,7 +7335,7 @@
         <v>7</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L25" s="12" t="s">
         <v>62</v>
@@ -7352,13 +7352,13 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>7</v>
@@ -7382,7 +7382,7 @@
         <v>7</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>62</v>
@@ -7399,13 +7399,13 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>7</v>
@@ -7429,7 +7429,7 @@
         <v>7</v>
       </c>
       <c r="K27" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L27" s="17" t="s">
         <v>67</v>
@@ -7446,13 +7446,13 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>7</v>
@@ -7476,7 +7476,7 @@
         <v>7</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L28" s="17" t="s">
         <v>30</v>
@@ -7493,13 +7493,13 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="13" t="s">
         <v>203</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>205</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>7</v>
@@ -7523,7 +7523,7 @@
         <v>7</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L29" s="17" t="s">
         <v>29</v>
@@ -7540,13 +7540,13 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B30" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>7</v>
@@ -7570,7 +7570,7 @@
         <v>7</v>
       </c>
       <c r="K30" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L30" s="17" t="s">
         <v>69</v>
@@ -7587,13 +7587,13 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B31" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>7</v>
@@ -7617,7 +7617,7 @@
         <v>7</v>
       </c>
       <c r="K31" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L31" s="17" t="s">
         <v>72</v>
@@ -7634,13 +7634,13 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B32" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>7</v>
@@ -7664,7 +7664,7 @@
         <v>7</v>
       </c>
       <c r="K32" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L32" s="17" t="s">
         <v>70</v>
@@ -7681,13 +7681,13 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B33" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>7</v>
@@ -7711,7 +7711,7 @@
         <v>7</v>
       </c>
       <c r="K33" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L33" s="12" t="s">
         <v>62</v>
@@ -7728,13 +7728,13 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B34" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>7</v>
@@ -7758,7 +7758,7 @@
         <v>7</v>
       </c>
       <c r="K34" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L34" s="12" t="s">
         <v>62</v>
@@ -7775,13 +7775,13 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B35" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>7</v>
@@ -7805,7 +7805,7 @@
         <v>7</v>
       </c>
       <c r="K35" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L35" s="12" t="s">
         <v>62</v>
@@ -7822,13 +7822,13 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B36" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>7</v>
@@ -7852,7 +7852,7 @@
         <v>7</v>
       </c>
       <c r="K36" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L36" s="12" t="s">
         <v>62</v>
@@ -7869,13 +7869,13 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B37" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>7</v>
@@ -7899,7 +7899,7 @@
         <v>7</v>
       </c>
       <c r="K37" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L37" s="12" t="s">
         <v>62</v>
@@ -7916,13 +7916,13 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B38" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>7</v>
@@ -7946,7 +7946,7 @@
         <v>7</v>
       </c>
       <c r="K38" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L38" s="12" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
update for debrief 1
</commit_message>
<xml_diff>
--- a/resources/DataLoginMenu.xlsx
+++ b/resources/DataLoginMenu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/G2Lab/FinalProject/QuotaAppTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0AF635-4D7E-364D-8854-0445CD7A9672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF73780-E843-444B-9E90-F87EC0D49FA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -637,9 +637,6 @@
     <t>positif case - valid phone number and email</t>
   </si>
   <si>
-    <t>testforgotpasswordbackend@gmail.com</t>
-  </si>
-  <si>
     <t>Length nama user must be less than 3 character</t>
   </si>
   <si>
@@ -652,16 +649,19 @@
     <t>Wrong otp</t>
   </si>
   <si>
-    <t>+6281252930391</t>
-  </si>
-  <si>
-    <t>+6281252930390</t>
-  </si>
-  <si>
-    <t>+6281252930392</t>
-  </si>
-  <si>
-    <t>testregisterbackend@gmail.com</t>
+    <t>+6281252930361</t>
+  </si>
+  <si>
+    <t>testregisterbackend23@gmail.com</t>
+  </si>
+  <si>
+    <t>+6281252930362</t>
+  </si>
+  <si>
+    <t>testforgotpasswordbackend23@gmail.com</t>
+  </si>
+  <si>
+    <t>+6281252930360</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1127,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1195,7 +1195,7 @@
         <v>56</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>25</v>
@@ -1212,7 +1212,7 @@
         <v>141</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>64</v>
@@ -1221,7 +1221,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1314,7 +1314,7 @@
         <v>45</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>66</v>
@@ -1331,7 +1331,7 @@
         <v>46</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>67</v>
@@ -1348,7 +1348,7 @@
         <v>60</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>28</v>
@@ -1365,7 +1365,7 @@
         <v>47</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>68</v>
@@ -1382,7 +1382,7 @@
         <v>48</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>70</v>
@@ -1399,7 +1399,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>69</v>
@@ -1421,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7189700-26BE-B342-926E-EF81568121D9}">
   <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O65" sqref="O65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1430,7 +1430,7 @@
     <col min="1" max="1" width="86.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.33203125" style="5" bestFit="1" customWidth="1"/>
@@ -1694,7 +1694,7 @@
         <v>167</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>30</v>
@@ -1741,7 +1741,7 @@
         <v>167</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>30</v>
@@ -1788,7 +1788,7 @@
         <v>167</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>64</v>
@@ -1835,7 +1835,7 @@
         <v>167</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>64</v>
@@ -1879,7 +1879,7 @@
         <v>145</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>24</v>
@@ -1926,7 +1926,7 @@
         <v>145</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>24</v>
@@ -1973,7 +1973,7 @@
         <v>145</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>24</v>
@@ -2020,7 +2020,7 @@
         <v>145</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>24</v>
@@ -2067,10 +2067,10 @@
         <v>145</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F14" s="17" t="s">
         <v>30</v>
@@ -2114,10 +2114,10 @@
         <v>145</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F15" s="17" t="s">
         <v>30</v>
@@ -2161,10 +2161,10 @@
         <v>145</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>64</v>
@@ -2208,10 +2208,10 @@
         <v>145</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>64</v>
@@ -2446,7 +2446,7 @@
         <v>167</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>30</v>
@@ -2493,7 +2493,7 @@
         <v>167</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F23" s="17" t="s">
         <v>30</v>
@@ -2540,7 +2540,7 @@
         <v>167</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>64</v>
@@ -2587,7 +2587,7 @@
         <v>167</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>64</v>
@@ -2631,7 +2631,7 @@
         <v>63</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E26" s="16" t="s">
         <v>24</v>
@@ -2678,7 +2678,7 @@
         <v>63</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>24</v>
@@ -2725,7 +2725,7 @@
         <v>63</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E28" s="16" t="s">
         <v>24</v>
@@ -2772,7 +2772,7 @@
         <v>63</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E29" s="16" t="s">
         <v>24</v>
@@ -2819,10 +2819,10 @@
         <v>63</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F30" s="17" t="s">
         <v>30</v>
@@ -2866,10 +2866,10 @@
         <v>63</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F31" s="17" t="s">
         <v>30</v>
@@ -2913,10 +2913,10 @@
         <v>63</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>64</v>
@@ -2960,10 +2960,10 @@
         <v>63</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>64</v>
@@ -3198,7 +3198,7 @@
         <v>167</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F38" s="17" t="s">
         <v>30</v>
@@ -3245,7 +3245,7 @@
         <v>167</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F39" s="17" t="s">
         <v>30</v>
@@ -3292,7 +3292,7 @@
         <v>167</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>64</v>
@@ -3339,7 +3339,7 @@
         <v>167</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>64</v>
@@ -3383,7 +3383,7 @@
         <v>145</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E42" s="16" t="s">
         <v>24</v>
@@ -3430,7 +3430,7 @@
         <v>145</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>24</v>
@@ -3477,7 +3477,7 @@
         <v>145</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E44" s="16" t="s">
         <v>24</v>
@@ -3524,7 +3524,7 @@
         <v>145</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E45" s="16" t="s">
         <v>24</v>
@@ -3571,10 +3571,10 @@
         <v>145</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F46" s="17" t="s">
         <v>30</v>
@@ -3618,10 +3618,10 @@
         <v>145</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>30</v>
@@ -3665,10 +3665,10 @@
         <v>145</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>64</v>
@@ -3712,10 +3712,10 @@
         <v>145</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>64</v>
@@ -3950,7 +3950,7 @@
         <v>167</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F54" s="17" t="s">
         <v>30</v>
@@ -3997,7 +3997,7 @@
         <v>167</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F55" s="17" t="s">
         <v>30</v>
@@ -4044,7 +4044,7 @@
         <v>167</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>64</v>
@@ -4091,7 +4091,7 @@
         <v>167</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F57" s="8" t="s">
         <v>64</v>
@@ -4135,7 +4135,7 @@
         <v>63</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>24</v>
@@ -4182,7 +4182,7 @@
         <v>63</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>24</v>
@@ -4229,7 +4229,7 @@
         <v>63</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>24</v>
@@ -4276,7 +4276,7 @@
         <v>63</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>24</v>
@@ -4323,10 +4323,10 @@
         <v>63</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F62" s="17" t="s">
         <v>30</v>
@@ -4370,10 +4370,10 @@
         <v>63</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F63" s="17" t="s">
         <v>30</v>
@@ -4417,10 +4417,10 @@
         <v>63</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>64</v>
@@ -4464,10 +4464,10 @@
         <v>63</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>64</v>
@@ -4497,7 +4497,7 @@
         <v>6</v>
       </c>
       <c r="O65" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
@@ -4511,10 +4511,10 @@
         <v>63</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>64</v>
@@ -4558,10 +4558,10 @@
         <v>63</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F67" s="8" t="s">
         <v>64</v>
@@ -4605,10 +4605,10 @@
         <v>63</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F68" s="8" t="s">
         <v>64</v>
@@ -4652,10 +4652,10 @@
         <v>57</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F69" s="8" t="s">
         <v>64</v>
@@ -4667,7 +4667,7 @@
         <v>22</v>
       </c>
       <c r="I69" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>20</v>
@@ -4699,10 +4699,10 @@
         <v>58</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F70" s="8" t="s">
         <v>64</v>
@@ -4746,10 +4746,10 @@
         <v>59</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F71" s="8" t="s">
         <v>64</v>
@@ -4796,7 +4796,7 @@
         <v>167</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F72" s="8" t="s">
         <v>64</v>
@@ -4840,7 +4840,7 @@
         <v>63</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E73" s="16" t="s">
         <v>24</v>
@@ -4887,7 +4887,7 @@
         <v>63</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E74" s="17" t="s">
         <v>143</v>
@@ -4902,7 +4902,7 @@
         <v>22</v>
       </c>
       <c r="I74" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>20</v>
@@ -4934,7 +4934,7 @@
         <v>63</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E75" s="17" t="s">
         <v>34</v>
@@ -4979,7 +4979,7 @@
         <v>63</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E76" s="17" t="s">
         <v>26</v>
@@ -5024,7 +5024,7 @@
         <v>63</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E77" s="17" t="s">
         <v>27</v>
@@ -5069,10 +5069,10 @@
         <v>63</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F78" s="17" t="s">
         <v>66</v>
@@ -5116,10 +5116,10 @@
         <v>63</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F79" s="17" t="s">
         <v>29</v>
@@ -5163,10 +5163,10 @@
         <v>63</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F80" s="17" t="s">
         <v>28</v>
@@ -5210,10 +5210,10 @@
         <v>63</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F81" s="17" t="s">
         <v>68</v>
@@ -5257,10 +5257,10 @@
         <v>63</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F82" s="17" t="s">
         <v>70</v>
@@ -5304,10 +5304,10 @@
         <v>63</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F83" s="17" t="s">
         <v>69</v>
@@ -5351,10 +5351,10 @@
         <v>63</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F84" s="8" t="s">
         <v>64</v>
@@ -5398,10 +5398,10 @@
         <v>63</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F85" s="8" t="s">
         <v>64</v>
@@ -5445,10 +5445,10 @@
         <v>63</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F86" s="8" t="s">
         <v>64</v>
@@ -5492,10 +5492,10 @@
         <v>63</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F87" s="8" t="s">
         <v>64</v>
@@ -5539,10 +5539,10 @@
         <v>63</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F88" s="8" t="s">
         <v>64</v>
@@ -5586,10 +5586,10 @@
         <v>63</v>
       </c>
       <c r="D89" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F89" s="8" t="s">
         <v>64</v>
@@ -5633,10 +5633,10 @@
         <v>63</v>
       </c>
       <c r="D90" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F90" s="8" t="s">
         <v>64</v>
@@ -5666,7 +5666,7 @@
         <v>22</v>
       </c>
       <c r="O90" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
@@ -5680,10 +5680,10 @@
         <v>63</v>
       </c>
       <c r="D91" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F91" s="8" t="s">
         <v>64</v>
@@ -5713,7 +5713,7 @@
         <v>22</v>
       </c>
       <c r="O91" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
@@ -5727,10 +5727,10 @@
         <v>63</v>
       </c>
       <c r="D92" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F92" s="8" t="s">
         <v>64</v>
@@ -5760,7 +5760,7 @@
         <v>22</v>
       </c>
       <c r="O92" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
@@ -5774,10 +5774,10 @@
         <v>63</v>
       </c>
       <c r="D93" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F93" s="8" t="s">
         <v>64</v>
@@ -5807,7 +5807,7 @@
         <v>6</v>
       </c>
       <c r="O93" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
@@ -5821,10 +5821,10 @@
         <v>63</v>
       </c>
       <c r="D94" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F94" s="8" t="s">
         <v>64</v>
@@ -5854,7 +5854,7 @@
         <v>22</v>
       </c>
       <c r="O94" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
@@ -5868,10 +5868,10 @@
         <v>63</v>
       </c>
       <c r="D95" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F95" s="8" t="s">
         <v>64</v>
@@ -5901,7 +5901,7 @@
         <v>22</v>
       </c>
       <c r="O95" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
@@ -5915,10 +5915,10 @@
         <v>63</v>
       </c>
       <c r="D96" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F96" s="8" t="s">
         <v>64</v>
@@ -5948,7 +5948,7 @@
         <v>22</v>
       </c>
       <c r="O96" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
@@ -5962,10 +5962,10 @@
         <v>63</v>
       </c>
       <c r="D97" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F97" s="8" t="s">
         <v>64</v>
@@ -5995,7 +5995,7 @@
         <v>22</v>
       </c>
       <c r="O97" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.2">
@@ -6009,10 +6009,10 @@
         <v>63</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F98" s="8" t="s">
         <v>64</v>
@@ -6042,7 +6042,7 @@
         <v>22</v>
       </c>
       <c r="O98" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
@@ -6056,10 +6056,10 @@
         <v>63</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F99" s="8" t="s">
         <v>64</v>
@@ -6089,7 +6089,7 @@
         <v>6</v>
       </c>
       <c r="O99" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.2">
@@ -6103,10 +6103,10 @@
         <v>63</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F100" s="8" t="s">
         <v>64</v>
@@ -6143,10 +6143,11 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1" xr:uid="{7C9F4664-0A34-C24D-816F-ED0CF82D64C6}"/>
-    <hyperlink ref="D11:D17" r:id="rId2" display="testregisterbackend@gmail.com" xr:uid="{CAC87F89-208F-364A-B7B7-20D1074E5F9B}"/>
-    <hyperlink ref="D26:D33" r:id="rId3" display="testregisterbackend@gmail.com" xr:uid="{8CBAC1EE-6A0D-8B43-A358-3A6B7EC25C05}"/>
-    <hyperlink ref="D42:D49" r:id="rId4" display="testregisterbackend@gmail.com" xr:uid="{19788135-A838-A446-8F7F-23D361E532F4}"/>
-    <hyperlink ref="D58:D71" r:id="rId5" display="testregisterbackend@gmail.com" xr:uid="{95E55E00-41D8-EF48-B25F-7124013393EF}"/>
+    <hyperlink ref="D11:D17" r:id="rId2" display="testregisterbackend23@gmail.com" xr:uid="{D1E88D9D-2F2D-DB40-A1DD-74F82724A49F}"/>
+    <hyperlink ref="D26:D33" r:id="rId3" display="testregisterbackend23@gmail.com" xr:uid="{650032F2-F814-0644-8437-E9288DB32EDB}"/>
+    <hyperlink ref="D42:D49" r:id="rId4" display="testregisterbackend23@gmail.com" xr:uid="{3F737BBF-4316-1848-87A7-D9D76C21C529}"/>
+    <hyperlink ref="D58:D71" r:id="rId5" display="testregisterbackend23@gmail.com" xr:uid="{7D6EB51B-218E-FE43-94D0-69E5220C4259}"/>
+    <hyperlink ref="D73:D100" r:id="rId6" display="testregisterbackend23@gmail.com" xr:uid="{3595A339-BA66-7140-ABDB-5961477650DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6156,15 +6157,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24BE3DA-8EEA-0F42-A704-7573A8A4E5B9}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="72.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
@@ -6281,7 +6282,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>22</v>
@@ -6325,7 +6326,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>166</v>
@@ -6372,10 +6373,10 @@
         <v>199</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>6</v>
@@ -6411,7 +6412,7 @@
         <v>6</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -6422,7 +6423,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>22</v>
@@ -6469,7 +6470,7 @@
         <v>143</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>22</v>
@@ -6516,7 +6517,7 @@
         <v>34</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>22</v>
@@ -6563,7 +6564,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>22</v>
@@ -6610,7 +6611,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>22</v>
@@ -6654,7 +6655,7 @@
         <v>40</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>166</v>
@@ -6701,10 +6702,10 @@
         <v>173</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>6</v>
@@ -6724,23 +6725,23 @@
       <c r="I12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="O12" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -6748,10 +6749,10 @@
         <v>32</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>6</v>
@@ -6771,23 +6772,23 @@
       <c r="I13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="K13" s="19" t="s">
+      <c r="O13" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -6795,10 +6796,10 @@
         <v>174</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>6</v>
@@ -6818,23 +6819,23 @@
       <c r="I14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="O14" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -6842,10 +6843,10 @@
         <v>175</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>6</v>
@@ -6881,7 +6882,7 @@
         <v>6</v>
       </c>
       <c r="O15" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -6889,10 +6890,10 @@
         <v>169</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>6</v>
@@ -6912,23 +6913,23 @@
       <c r="I16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="18" t="s">
+      <c r="J16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="O16" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -6936,10 +6937,10 @@
         <v>170</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>6</v>
@@ -6959,23 +6960,23 @@
       <c r="I17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="18" t="s">
+      <c r="J17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="O17" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O17" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -6983,10 +6984,10 @@
         <v>171</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>6</v>
@@ -7006,23 +7007,23 @@
       <c r="I18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="18" t="s">
+      <c r="J18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N18" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="O18" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -7030,10 +7031,10 @@
         <v>172</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>6</v>
@@ -7053,23 +7054,23 @@
       <c r="I19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="18" t="s">
+      <c r="J19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N19" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="K19" s="19" t="s">
+      <c r="O19" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O19" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -7077,10 +7078,10 @@
         <v>32</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>6</v>
@@ -7100,23 +7101,23 @@
       <c r="I20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="J20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N20" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="O20" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -7124,10 +7125,10 @@
         <v>176</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>6</v>
@@ -7163,7 +7164,7 @@
         <v>6</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -7171,10 +7172,10 @@
         <v>33</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>6</v>
@@ -7218,10 +7219,10 @@
         <v>182</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>6</v>
@@ -7238,14 +7239,14 @@
       <c r="H23" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>165</v>
+      <c r="I23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L23" s="18" t="s">
         <v>68</v>
@@ -7265,10 +7266,10 @@
         <v>184</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>6</v>
@@ -7285,14 +7286,14 @@
       <c r="H24" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>165</v>
+      <c r="I24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L24" s="18" t="s">
         <v>68</v>
@@ -7312,10 +7313,10 @@
         <v>183</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>6</v>
@@ -7332,14 +7333,14 @@
       <c r="H25" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>165</v>
+      <c r="I25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L25" s="12" t="s">
         <v>61</v>
@@ -7359,10 +7360,10 @@
         <v>185</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>6</v>
@@ -7373,20 +7374,20 @@
       <c r="F26" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" s="10" t="s">
+      <c r="G26" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K26" s="14" t="s">
-        <v>165</v>
+      <c r="H26" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>61</v>
@@ -7398,7 +7399,7 @@
         <v>6</v>
       </c>
       <c r="O26" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
@@ -7406,10 +7407,10 @@
         <v>187</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>6</v>
@@ -7420,20 +7421,20 @@
       <c r="F27" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="10" t="s">
+      <c r="G27" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J27" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K27" s="14" t="s">
-        <v>165</v>
+      <c r="H27" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L27" s="17" t="s">
         <v>66</v>
@@ -7453,10 +7454,10 @@
         <v>188</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>6</v>
@@ -7467,20 +7468,20 @@
       <c r="F28" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I28" s="10" t="s">
+      <c r="G28" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J28" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K28" s="14" t="s">
-        <v>165</v>
+      <c r="H28" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L28" s="17" t="s">
         <v>29</v>
@@ -7500,10 +7501,10 @@
         <v>198</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>6</v>
@@ -7514,20 +7515,20 @@
       <c r="F29" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G29" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" s="10" t="s">
+      <c r="G29" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J29" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K29" s="14" t="s">
-        <v>165</v>
+      <c r="H29" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L29" s="17" t="s">
         <v>28</v>
@@ -7547,10 +7548,10 @@
         <v>189</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>6</v>
@@ -7561,20 +7562,20 @@
       <c r="F30" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G30" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I30" s="10" t="s">
+      <c r="G30" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J30" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K30" s="14" t="s">
-        <v>165</v>
+      <c r="H30" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L30" s="17" t="s">
         <v>68</v>
@@ -7594,10 +7595,10 @@
         <v>190</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>6</v>
@@ -7608,20 +7609,20 @@
       <c r="F31" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I31" s="10" t="s">
+      <c r="G31" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J31" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K31" s="14" t="s">
-        <v>165</v>
+      <c r="H31" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L31" s="17" t="s">
         <v>70</v>
@@ -7641,10 +7642,10 @@
         <v>191</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>6</v>
@@ -7655,20 +7656,20 @@
       <c r="F32" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32" s="10" t="s">
+      <c r="G32" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J32" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K32" s="14" t="s">
-        <v>165</v>
+      <c r="H32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L32" s="17" t="s">
         <v>69</v>
@@ -7688,10 +7689,10 @@
         <v>192</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>6</v>
@@ -7702,20 +7703,20 @@
       <c r="F33" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I33" s="10" t="s">
+      <c r="G33" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J33" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K33" s="14" t="s">
-        <v>165</v>
+      <c r="H33" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L33" s="12" t="s">
         <v>61</v>
@@ -7735,10 +7736,10 @@
         <v>193</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>6</v>
@@ -7749,20 +7750,20 @@
       <c r="F34" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G34" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I34" s="10" t="s">
+      <c r="G34" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J34" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K34" s="14" t="s">
-        <v>165</v>
+      <c r="H34" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L34" s="12" t="s">
         <v>61</v>
@@ -7782,10 +7783,10 @@
         <v>194</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>6</v>
@@ -7796,20 +7797,20 @@
       <c r="F35" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I35" s="10" t="s">
+      <c r="G35" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K35" s="14" t="s">
-        <v>165</v>
+      <c r="H35" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L35" s="12" t="s">
         <v>61</v>
@@ -7829,10 +7830,10 @@
         <v>195</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>6</v>
@@ -7843,20 +7844,20 @@
       <c r="F36" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I36" s="10" t="s">
+      <c r="G36" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J36" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K36" s="14" t="s">
-        <v>165</v>
+      <c r="H36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L36" s="12" t="s">
         <v>61</v>
@@ -7876,10 +7877,10 @@
         <v>196</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>6</v>
@@ -7890,20 +7891,20 @@
       <c r="F37" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G37" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I37" s="10" t="s">
+      <c r="G37" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J37" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K37" s="14" t="s">
-        <v>165</v>
+      <c r="H37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L37" s="12" t="s">
         <v>61</v>
@@ -7923,10 +7924,10 @@
         <v>197</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>6</v>
@@ -7937,20 +7938,20 @@
       <c r="F38" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G38" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I38" s="10" t="s">
+      <c r="G38" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J38" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K38" s="14" t="s">
-        <v>165</v>
+      <c r="H38" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L38" s="12" t="s">
         <v>61</v>
@@ -7968,9 +7969,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{0B31C92F-2BAF-F340-8F62-35582DE47EEB}"/>
-    <hyperlink ref="C5:C10" r:id="rId2" display="testforgotpasswordbackend@gmail.com" xr:uid="{CD3AD3A9-B85E-C141-9022-FBE84B40036A}"/>
-    <hyperlink ref="C12:C38" r:id="rId3" display="testforgotpasswordbackend@gmail.com" xr:uid="{F6DC4111-2015-8643-A854-CC53345C986F}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{C9F2683C-21BB-1C46-A6EC-94FD665ED47D}"/>
+    <hyperlink ref="C5:C10" r:id="rId2" display="testforgotpasswordbackend23@gmail.com" xr:uid="{FCE07073-61CE-F245-85EA-C325A7FC9502}"/>
+    <hyperlink ref="C12:C38" r:id="rId3" display="testforgotpasswordbackend23@gmail.com" xr:uid="{D221E23F-469D-7A4E-AD35-38F3169ED136}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update login dan delete account
</commit_message>
<xml_diff>
--- a/resources/DataLoginMenu.xlsx
+++ b/resources/DataLoginMenu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/G2Lab/FinalProject/QuotaAppTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF73780-E843-444B-9E90-F87EC0D49FA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612BF7D9-34EC-5D48-8DE9-248594C69F64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -1421,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7189700-26BE-B342-926E-EF81568121D9}">
   <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O65" sqref="O65"/>
+    <sheetView tabSelected="1" topLeftCell="I69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N92" sqref="N92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6157,7 +6157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24BE3DA-8EEA-0F42-A704-7573A8A4E5B9}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixing with mentors advices
</commit_message>
<xml_diff>
--- a/resources/DataLoginMenu.xlsx
+++ b/resources/DataLoginMenu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/G2Lab/FinalProject/QuotaAppTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612BF7D9-34EC-5D48-8DE9-248594C69F64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A753E4-9BD1-0244-8830-BF3E103F38C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="212">
   <si>
     <t>password</t>
   </si>
@@ -469,9 +469,6 @@
     <t>+628123456789101112222</t>
   </si>
   <si>
-    <t>size must be between 0 and 20</t>
-  </si>
-  <si>
     <t>12345678</t>
   </si>
   <si>
@@ -662,6 +659,18 @@
   </si>
   <si>
     <t>+6281252930360</t>
+  </si>
+  <si>
+    <t>+6281252930362 ----</t>
+  </si>
+  <si>
+    <t>signup is successfully</t>
+  </si>
+  <si>
+    <t>No message available</t>
+  </si>
+  <si>
+    <t>successfully</t>
   </si>
 </sst>
 </file>
@@ -1126,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9959BB-4BD4-1645-834F-8040D5B979C6}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1170,7 +1179,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1187,7 +1196,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1195,7 +1204,7 @@
         <v>56</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>25</v>
@@ -1212,7 +1221,7 @@
         <v>141</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>64</v>
@@ -1221,7 +1230,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1238,7 +1247,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1255,7 +1264,7 @@
         <v>22</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1272,7 +1281,7 @@
         <v>22</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1289,7 +1298,7 @@
         <v>22</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1306,7 +1315,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1314,7 +1323,7 @@
         <v>45</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>66</v>
@@ -1331,7 +1340,7 @@
         <v>46</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>67</v>
@@ -1348,7 +1357,7 @@
         <v>60</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>28</v>
@@ -1365,7 +1374,7 @@
         <v>47</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>68</v>
@@ -1382,7 +1391,7 @@
         <v>48</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>70</v>
@@ -1399,7 +1408,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>69</v>
@@ -1421,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7189700-26BE-B342-926E-EF81568121D9}">
   <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N92" sqref="N92"/>
+    <sheetView topLeftCell="E52" zoomScale="103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1486,7 +1495,7 @@
         <v>3</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>15</v>
@@ -1500,10 +1509,10 @@
         <v>74</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>24</v>
@@ -1512,13 +1521,13 @@
         <v>30</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>20</v>
@@ -1547,10 +1556,10 @@
         <v>74</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>24</v>
@@ -1565,7 +1574,7 @@
         <v>22</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>20</v>
@@ -1594,10 +1603,10 @@
         <v>74</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>24</v>
@@ -1606,13 +1615,13 @@
         <v>64</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H4" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>20</v>
@@ -1641,10 +1650,10 @@
         <v>74</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>24</v>
@@ -1659,7 +1668,7 @@
         <v>22</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>20</v>
@@ -1688,25 +1697,25 @@
         <v>74</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>30</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>20</v>
@@ -1735,13 +1744,13 @@
         <v>74</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>30</v>
@@ -1753,7 +1762,7 @@
         <v>22</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>20</v>
@@ -1782,25 +1791,25 @@
         <v>74</v>
       </c>
       <c r="C8" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>146</v>
-      </c>
       <c r="H8" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>20</v>
@@ -1829,13 +1838,13 @@
         <v>74</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>64</v>
@@ -1847,7 +1856,7 @@
         <v>22</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>20</v>
@@ -1876,10 +1885,10 @@
         <v>74</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>24</v>
@@ -1888,13 +1897,13 @@
         <v>30</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>20</v>
@@ -1923,10 +1932,10 @@
         <v>74</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>24</v>
@@ -1941,7 +1950,7 @@
         <v>22</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>20</v>
@@ -1970,10 +1979,10 @@
         <v>74</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>24</v>
@@ -1982,13 +1991,13 @@
         <v>64</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>20</v>
@@ -2017,10 +2026,10 @@
         <v>74</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>24</v>
@@ -2035,7 +2044,7 @@
         <v>22</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>20</v>
@@ -2064,25 +2073,25 @@
         <v>74</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D14" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H14" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>20</v>
@@ -2111,13 +2120,13 @@
         <v>74</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D15" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F15" s="17" t="s">
         <v>30</v>
@@ -2129,7 +2138,7 @@
         <v>22</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>20</v>
@@ -2158,25 +2167,25 @@
         <v>74</v>
       </c>
       <c r="C16" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>146</v>
-      </c>
       <c r="H16" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>20</v>
@@ -2205,14 +2214,14 @@
         <v>74</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D17" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="F17" s="8" t="s">
         <v>64</v>
       </c>
@@ -2223,7 +2232,7 @@
         <v>22</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>20</v>
@@ -2255,7 +2264,7 @@
         <v>63</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>24</v>
@@ -2264,13 +2273,13 @@
         <v>30</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H18" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>20</v>
@@ -2302,7 +2311,7 @@
         <v>63</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>24</v>
@@ -2317,7 +2326,7 @@
         <v>22</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>20</v>
@@ -2349,7 +2358,7 @@
         <v>63</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>24</v>
@@ -2358,13 +2367,13 @@
         <v>64</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H20" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>20</v>
@@ -2396,7 +2405,7 @@
         <v>63</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E21" s="16" t="s">
         <v>24</v>
@@ -2411,7 +2420,7 @@
         <v>22</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>20</v>
@@ -2443,22 +2452,22 @@
         <v>63</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>30</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>20</v>
@@ -2490,10 +2499,10 @@
         <v>63</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F23" s="17" t="s">
         <v>30</v>
@@ -2505,7 +2514,7 @@
         <v>22</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>20</v>
@@ -2537,22 +2546,22 @@
         <v>63</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>64</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H24" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>20</v>
@@ -2584,10 +2593,10 @@
         <v>63</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>64</v>
@@ -2599,7 +2608,7 @@
         <v>22</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>20</v>
@@ -2631,7 +2640,7 @@
         <v>63</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E26" s="16" t="s">
         <v>24</v>
@@ -2640,13 +2649,13 @@
         <v>30</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H26" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>20</v>
@@ -2678,7 +2687,7 @@
         <v>63</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>24</v>
@@ -2693,7 +2702,7 @@
         <v>22</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>20</v>
@@ -2725,7 +2734,7 @@
         <v>63</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E28" s="16" t="s">
         <v>24</v>
@@ -2734,13 +2743,13 @@
         <v>64</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H28" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>20</v>
@@ -2772,7 +2781,7 @@
         <v>63</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E29" s="16" t="s">
         <v>24</v>
@@ -2787,7 +2796,7 @@
         <v>22</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>20</v>
@@ -2819,22 +2828,22 @@
         <v>63</v>
       </c>
       <c r="D30" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F30" s="17" t="s">
         <v>30</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H30" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>20</v>
@@ -2866,10 +2875,10 @@
         <v>63</v>
       </c>
       <c r="D31" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F31" s="17" t="s">
         <v>30</v>
@@ -2881,7 +2890,7 @@
         <v>22</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>20</v>
@@ -2913,22 +2922,22 @@
         <v>63</v>
       </c>
       <c r="D32" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E32" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="F32" s="8" t="s">
         <v>64</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H32" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>20</v>
@@ -2960,11 +2969,11 @@
         <v>63</v>
       </c>
       <c r="D33" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E33" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="F33" s="8" t="s">
         <v>64</v>
       </c>
@@ -2975,7 +2984,7 @@
         <v>22</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>20</v>
@@ -3004,10 +3013,10 @@
         <v>75</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E34" s="16" t="s">
         <v>24</v>
@@ -3016,13 +3025,13 @@
         <v>30</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H34" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>20</v>
@@ -3051,10 +3060,10 @@
         <v>75</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E35" s="16" t="s">
         <v>24</v>
@@ -3069,7 +3078,7 @@
         <v>22</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>20</v>
@@ -3098,10 +3107,10 @@
         <v>75</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E36" s="16" t="s">
         <v>24</v>
@@ -3110,13 +3119,13 @@
         <v>64</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H36" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>20</v>
@@ -3145,10 +3154,10 @@
         <v>75</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E37" s="16" t="s">
         <v>24</v>
@@ -3163,7 +3172,7 @@
         <v>22</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>20</v>
@@ -3192,25 +3201,25 @@
         <v>75</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F38" s="17" t="s">
         <v>30</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H38" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>20</v>
@@ -3239,13 +3248,13 @@
         <v>75</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F39" s="17" t="s">
         <v>30</v>
@@ -3257,7 +3266,7 @@
         <v>22</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>20</v>
@@ -3286,25 +3295,25 @@
         <v>75</v>
       </c>
       <c r="C40" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>146</v>
-      </c>
       <c r="H40" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>20</v>
@@ -3333,13 +3342,13 @@
         <v>75</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>64</v>
@@ -3351,7 +3360,7 @@
         <v>22</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>20</v>
@@ -3380,10 +3389,10 @@
         <v>75</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E42" s="16" t="s">
         <v>24</v>
@@ -3392,13 +3401,13 @@
         <v>30</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H42" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I42" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>20</v>
@@ -3427,10 +3436,10 @@
         <v>75</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>24</v>
@@ -3445,7 +3454,7 @@
         <v>22</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>20</v>
@@ -3474,10 +3483,10 @@
         <v>75</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E44" s="16" t="s">
         <v>24</v>
@@ -3486,13 +3495,13 @@
         <v>64</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H44" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I44" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>20</v>
@@ -3521,10 +3530,10 @@
         <v>75</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E45" s="16" t="s">
         <v>24</v>
@@ -3539,7 +3548,7 @@
         <v>22</v>
       </c>
       <c r="I45" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>20</v>
@@ -3568,25 +3577,25 @@
         <v>75</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D46" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E46" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F46" s="17" t="s">
         <v>30</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H46" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I46" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>20</v>
@@ -3615,13 +3624,13 @@
         <v>75</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D47" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E47" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>30</v>
@@ -3633,7 +3642,7 @@
         <v>22</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>20</v>
@@ -3662,25 +3671,25 @@
         <v>75</v>
       </c>
       <c r="C48" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G48" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G48" s="17" t="s">
-        <v>146</v>
-      </c>
       <c r="H48" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I48" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>20</v>
@@ -3709,14 +3718,14 @@
         <v>75</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D49" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E49" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E49" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="F49" s="8" t="s">
         <v>64</v>
       </c>
@@ -3727,7 +3736,7 @@
         <v>22</v>
       </c>
       <c r="I49" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>20</v>
@@ -3759,7 +3768,7 @@
         <v>63</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E50" s="16" t="s">
         <v>24</v>
@@ -3768,13 +3777,13 @@
         <v>30</v>
       </c>
       <c r="G50" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H50" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I50" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>20</v>
@@ -3806,7 +3815,7 @@
         <v>63</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E51" s="16" t="s">
         <v>24</v>
@@ -3821,7 +3830,7 @@
         <v>22</v>
       </c>
       <c r="I51" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>20</v>
@@ -3853,7 +3862,7 @@
         <v>63</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>24</v>
@@ -3862,13 +3871,13 @@
         <v>64</v>
       </c>
       <c r="G52" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H52" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I52" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>20</v>
@@ -3900,7 +3909,7 @@
         <v>63</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>24</v>
@@ -3915,7 +3924,7 @@
         <v>22</v>
       </c>
       <c r="I53" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>20</v>
@@ -3947,22 +3956,22 @@
         <v>63</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F54" s="17" t="s">
         <v>30</v>
       </c>
       <c r="G54" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H54" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I54" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>20</v>
@@ -3994,10 +4003,10 @@
         <v>63</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F55" s="17" t="s">
         <v>30</v>
@@ -4009,7 +4018,7 @@
         <v>22</v>
       </c>
       <c r="I55" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>20</v>
@@ -4041,22 +4050,22 @@
         <v>63</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>64</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H56" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I56" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>20</v>
@@ -4088,10 +4097,10 @@
         <v>63</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F57" s="8" t="s">
         <v>64</v>
@@ -4103,7 +4112,7 @@
         <v>22</v>
       </c>
       <c r="I57" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>20</v>
@@ -4135,7 +4144,7 @@
         <v>63</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>24</v>
@@ -4144,13 +4153,13 @@
         <v>30</v>
       </c>
       <c r="G58" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H58" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I58" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>20</v>
@@ -4182,7 +4191,7 @@
         <v>63</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>24</v>
@@ -4197,7 +4206,7 @@
         <v>22</v>
       </c>
       <c r="I59" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>20</v>
@@ -4229,7 +4238,7 @@
         <v>63</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>24</v>
@@ -4238,13 +4247,13 @@
         <v>64</v>
       </c>
       <c r="G60" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H60" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I60" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>20</v>
@@ -4276,7 +4285,7 @@
         <v>63</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>24</v>
@@ -4291,7 +4300,7 @@
         <v>22</v>
       </c>
       <c r="I61" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>20</v>
@@ -4323,22 +4332,22 @@
         <v>63</v>
       </c>
       <c r="D62" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E62" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F62" s="17" t="s">
         <v>30</v>
       </c>
       <c r="G62" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H62" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I62" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>20</v>
@@ -4370,10 +4379,10 @@
         <v>63</v>
       </c>
       <c r="D63" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E63" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F63" s="17" t="s">
         <v>30</v>
@@ -4385,7 +4394,7 @@
         <v>22</v>
       </c>
       <c r="I63" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>20</v>
@@ -4417,22 +4426,22 @@
         <v>63</v>
       </c>
       <c r="D64" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E64" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E64" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="F64" s="8" t="s">
         <v>64</v>
       </c>
       <c r="G64" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H64" s="16" t="s">
         <v>22</v>
       </c>
       <c r="I64" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>20</v>
@@ -4464,10 +4473,10 @@
         <v>63</v>
       </c>
       <c r="D65" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E65" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>64</v>
@@ -4479,7 +4488,7 @@
         <v>6</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="J65" s="12" t="s">
         <v>17</v>
@@ -4497,7 +4506,7 @@
         <v>6</v>
       </c>
       <c r="O65" s="8" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
@@ -4511,11 +4520,11 @@
         <v>63</v>
       </c>
       <c r="D66" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E66" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E66" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="F66" s="8" t="s">
         <v>64</v>
       </c>
@@ -4526,7 +4535,7 @@
         <v>22</v>
       </c>
       <c r="I66" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>20</v>
@@ -4558,11 +4567,11 @@
         <v>63</v>
       </c>
       <c r="D67" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E67" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E67" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="F67" s="8" t="s">
         <v>64</v>
       </c>
@@ -4573,7 +4582,7 @@
         <v>22</v>
       </c>
       <c r="I67" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J67" s="4" t="s">
         <v>20</v>
@@ -4605,11 +4614,11 @@
         <v>63</v>
       </c>
       <c r="D68" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E68" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E68" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="F68" s="8" t="s">
         <v>64</v>
       </c>
@@ -4620,7 +4629,7 @@
         <v>22</v>
       </c>
       <c r="I68" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>20</v>
@@ -4652,11 +4661,11 @@
         <v>57</v>
       </c>
       <c r="D69" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E69" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E69" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="F69" s="8" t="s">
         <v>64</v>
       </c>
@@ -4667,7 +4676,7 @@
         <v>22</v>
       </c>
       <c r="I69" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>20</v>
@@ -4699,11 +4708,11 @@
         <v>58</v>
       </c>
       <c r="D70" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E70" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E70" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="F70" s="8" t="s">
         <v>64</v>
       </c>
@@ -4713,9 +4722,7 @@
       <c r="H70" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I70" s="16" t="s">
-        <v>144</v>
-      </c>
+      <c r="I70" s="16"/>
       <c r="J70" s="4" t="s">
         <v>20</v>
       </c>
@@ -4746,11 +4753,11 @@
         <v>59</v>
       </c>
       <c r="D71" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E71" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E71" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="F71" s="8" t="s">
         <v>64</v>
       </c>
@@ -4761,7 +4768,7 @@
         <v>22</v>
       </c>
       <c r="I71" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>20</v>
@@ -4793,10 +4800,10 @@
         <v>63</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F72" s="8" t="s">
         <v>64</v>
@@ -4808,7 +4815,7 @@
         <v>22</v>
       </c>
       <c r="I72" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>20</v>
@@ -4840,7 +4847,7 @@
         <v>63</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E73" s="16" t="s">
         <v>24</v>
@@ -4855,7 +4862,7 @@
         <v>22</v>
       </c>
       <c r="I73" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>20</v>
@@ -4887,7 +4894,7 @@
         <v>63</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E74" s="17" t="s">
         <v>143</v>
@@ -4902,7 +4909,7 @@
         <v>22</v>
       </c>
       <c r="I74" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>20</v>
@@ -4934,7 +4941,7 @@
         <v>63</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E75" s="17" t="s">
         <v>34</v>
@@ -4970,7 +4977,7 @@
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B76" s="10" t="s">
         <v>75</v>
@@ -4979,7 +4986,7 @@
         <v>63</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E76" s="17" t="s">
         <v>26</v>
@@ -5024,7 +5031,7 @@
         <v>63</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E77" s="17" t="s">
         <v>27</v>
@@ -5069,10 +5076,10 @@
         <v>63</v>
       </c>
       <c r="D78" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E78" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F78" s="17" t="s">
         <v>66</v>
@@ -5084,7 +5091,7 @@
         <v>22</v>
       </c>
       <c r="I78" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J78" s="4" t="s">
         <v>20</v>
@@ -5116,10 +5123,10 @@
         <v>63</v>
       </c>
       <c r="D79" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E79" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E79" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F79" s="17" t="s">
         <v>29</v>
@@ -5131,7 +5138,7 @@
         <v>22</v>
       </c>
       <c r="I79" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>20</v>
@@ -5163,10 +5170,10 @@
         <v>63</v>
       </c>
       <c r="D80" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E80" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E80" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F80" s="17" t="s">
         <v>28</v>
@@ -5178,7 +5185,7 @@
         <v>22</v>
       </c>
       <c r="I80" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J80" s="4" t="s">
         <v>20</v>
@@ -5210,10 +5217,10 @@
         <v>63</v>
       </c>
       <c r="D81" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E81" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E81" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F81" s="17" t="s">
         <v>68</v>
@@ -5257,10 +5264,10 @@
         <v>63</v>
       </c>
       <c r="D82" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E82" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F82" s="17" t="s">
         <v>70</v>
@@ -5304,10 +5311,10 @@
         <v>63</v>
       </c>
       <c r="D83" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E83" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F83" s="17" t="s">
         <v>69</v>
@@ -5351,10 +5358,10 @@
         <v>63</v>
       </c>
       <c r="D84" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E84" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F84" s="8" t="s">
         <v>64</v>
@@ -5366,7 +5373,7 @@
         <v>22</v>
       </c>
       <c r="I84" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J84" s="4" t="s">
         <v>20</v>
@@ -5398,10 +5405,10 @@
         <v>63</v>
       </c>
       <c r="D85" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E85" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E85" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F85" s="8" t="s">
         <v>64</v>
@@ -5413,7 +5420,7 @@
         <v>22</v>
       </c>
       <c r="I85" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J85" s="4" t="s">
         <v>20</v>
@@ -5445,10 +5452,10 @@
         <v>63</v>
       </c>
       <c r="D86" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E86" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E86" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F86" s="8" t="s">
         <v>64</v>
@@ -5460,7 +5467,7 @@
         <v>22</v>
       </c>
       <c r="I86" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J86" s="4" t="s">
         <v>20</v>
@@ -5492,10 +5499,10 @@
         <v>63</v>
       </c>
       <c r="D87" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E87" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E87" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F87" s="8" t="s">
         <v>64</v>
@@ -5507,7 +5514,7 @@
         <v>22</v>
       </c>
       <c r="I87" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J87" s="4" t="s">
         <v>20</v>
@@ -5539,10 +5546,10 @@
         <v>63</v>
       </c>
       <c r="D88" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E88" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E88" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F88" s="8" t="s">
         <v>64</v>
@@ -5554,7 +5561,7 @@
         <v>22</v>
       </c>
       <c r="I88" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J88" s="4" t="s">
         <v>20</v>
@@ -5586,10 +5593,10 @@
         <v>63</v>
       </c>
       <c r="D89" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E89" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E89" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F89" s="8" t="s">
         <v>64</v>
@@ -5601,7 +5608,7 @@
         <v>22</v>
       </c>
       <c r="I89" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J89" s="4" t="s">
         <v>20</v>
@@ -5624,7 +5631,7 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B90" s="10" t="s">
         <v>75</v>
@@ -5633,10 +5640,10 @@
         <v>63</v>
       </c>
       <c r="D90" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E90" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E90" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F90" s="8" t="s">
         <v>64</v>
@@ -5648,13 +5655,13 @@
         <v>6</v>
       </c>
       <c r="I90" s="12" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="J90" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K90" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L90" s="18" t="s">
         <v>5</v>
@@ -5666,7 +5673,7 @@
         <v>22</v>
       </c>
       <c r="O90" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
@@ -5680,10 +5687,10 @@
         <v>63</v>
       </c>
       <c r="D91" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E91" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E91" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F91" s="8" t="s">
         <v>64</v>
@@ -5695,13 +5702,13 @@
         <v>6</v>
       </c>
       <c r="I91" s="12" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="J91" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K91" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L91" s="12" t="s">
         <v>4</v>
@@ -5713,12 +5720,12 @@
         <v>22</v>
       </c>
       <c r="O91" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B92" s="10" t="s">
         <v>75</v>
@@ -5727,10 +5734,10 @@
         <v>63</v>
       </c>
       <c r="D92" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E92" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E92" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F92" s="8" t="s">
         <v>64</v>
@@ -5742,7 +5749,7 @@
         <v>6</v>
       </c>
       <c r="I92" s="12" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="J92" s="1" t="s">
         <v>17</v>
@@ -5760,12 +5767,12 @@
         <v>22</v>
       </c>
       <c r="O92" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B93" s="10" t="s">
         <v>75</v>
@@ -5774,10 +5781,10 @@
         <v>63</v>
       </c>
       <c r="D93" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E93" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E93" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F93" s="8" t="s">
         <v>64</v>
@@ -5789,7 +5796,7 @@
         <v>6</v>
       </c>
       <c r="I93" s="12" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="J93" s="12" t="s">
         <v>17</v>
@@ -5807,12 +5814,12 @@
         <v>6</v>
       </c>
       <c r="O93" s="8" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B94" s="10" t="s">
         <v>75</v>
@@ -5821,10 +5828,10 @@
         <v>63</v>
       </c>
       <c r="D94" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E94" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E94" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F94" s="8" t="s">
         <v>64</v>
@@ -5836,13 +5843,13 @@
         <v>6</v>
       </c>
       <c r="I94" s="12" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="J94" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K94" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L94" s="12" t="s">
         <v>4</v>
@@ -5854,12 +5861,12 @@
         <v>22</v>
       </c>
       <c r="O94" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B95" s="10" t="s">
         <v>75</v>
@@ -5868,10 +5875,10 @@
         <v>63</v>
       </c>
       <c r="D95" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E95" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E95" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F95" s="8" t="s">
         <v>64</v>
@@ -5883,13 +5890,13 @@
         <v>6</v>
       </c>
       <c r="I95" s="12" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="J95" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K95" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L95" s="12" t="s">
         <v>4</v>
@@ -5901,12 +5908,12 @@
         <v>22</v>
       </c>
       <c r="O95" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>75</v>
@@ -5915,10 +5922,10 @@
         <v>63</v>
       </c>
       <c r="D96" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E96" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F96" s="8" t="s">
         <v>64</v>
@@ -5930,13 +5937,13 @@
         <v>6</v>
       </c>
       <c r="I96" s="12" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K96" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L96" s="12" t="s">
         <v>4</v>
@@ -5948,12 +5955,12 @@
         <v>22</v>
       </c>
       <c r="O96" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B97" s="10" t="s">
         <v>75</v>
@@ -5962,10 +5969,10 @@
         <v>63</v>
       </c>
       <c r="D97" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E97" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F97" s="8" t="s">
         <v>64</v>
@@ -5977,7 +5984,7 @@
         <v>6</v>
       </c>
       <c r="I97" s="12" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="J97" s="1" t="s">
         <v>17</v>
@@ -5995,7 +6002,7 @@
         <v>22</v>
       </c>
       <c r="O97" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.2">
@@ -6009,10 +6016,10 @@
         <v>63</v>
       </c>
       <c r="D98" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E98" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F98" s="8" t="s">
         <v>64</v>
@@ -6024,13 +6031,13 @@
         <v>6</v>
       </c>
       <c r="I98" s="12" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K98" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L98" s="12" t="s">
         <v>4</v>
@@ -6042,12 +6049,12 @@
         <v>22</v>
       </c>
       <c r="O98" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B99" s="10" t="s">
         <v>75</v>
@@ -6056,10 +6063,10 @@
         <v>63</v>
       </c>
       <c r="D99" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E99" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F99" s="8" t="s">
         <v>64</v>
@@ -6071,7 +6078,7 @@
         <v>6</v>
       </c>
       <c r="I99" s="12" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="J99" s="4" t="s">
         <v>18</v>
@@ -6089,7 +6096,7 @@
         <v>6</v>
       </c>
       <c r="O99" s="8" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.2">
@@ -6103,10 +6110,10 @@
         <v>63</v>
       </c>
       <c r="D100" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E100" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="F100" s="8" t="s">
         <v>64</v>
@@ -6118,7 +6125,7 @@
         <v>6</v>
       </c>
       <c r="I100" s="12" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="J100" s="4" t="s">
         <v>18</v>
@@ -6130,13 +6137,13 @@
         <v>20</v>
       </c>
       <c r="M100" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N100" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O100" s="19" t="s">
-        <v>148</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -6150,6 +6157,7 @@
     <hyperlink ref="D73:D100" r:id="rId6" display="testregisterbackend23@gmail.com" xr:uid="{3595A339-BA66-7140-ABDB-5961477650DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6209,22 +6217,22 @@
         <v>3</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>15</v>
       </c>
       <c r="L1" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="M1" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="N1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>160</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -6235,13 +6243,13 @@
         <v>24</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D2" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>148</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>20</v>
@@ -6282,13 +6290,13 @@
         <v>24</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>20</v>
@@ -6326,16 +6334,16 @@
         <v>35</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D4" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>148</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>20</v>
@@ -6370,13 +6378,13 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>6</v>
@@ -6400,7 +6408,7 @@
         <v>6</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L5" s="12" t="s">
         <v>61</v>
@@ -6412,7 +6420,7 @@
         <v>6</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -6423,13 +6431,13 @@
         <v>24</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>20</v>
@@ -6470,13 +6478,13 @@
         <v>143</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>20</v>
@@ -6517,13 +6525,13 @@
         <v>34</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>20</v>
@@ -6564,13 +6572,13 @@
         <v>26</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>20</v>
@@ -6611,13 +6619,13 @@
         <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>20</v>
@@ -6655,16 +6663,16 @@
         <v>40</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D11" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>148</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>20</v>
@@ -6699,13 +6707,13 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>6</v>
@@ -6717,7 +6725,7 @@
         <v>17</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>5</v>
@@ -6738,10 +6746,10 @@
         <v>20</v>
       </c>
       <c r="N12" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="O12" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="O12" s="19" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -6749,10 +6757,10 @@
         <v>32</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>6</v>
@@ -6764,7 +6772,7 @@
         <v>17</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>4</v>
@@ -6785,21 +6793,21 @@
         <v>20</v>
       </c>
       <c r="N13" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="O13" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="O13" s="19" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>6</v>
@@ -6832,21 +6840,21 @@
         <v>20</v>
       </c>
       <c r="N14" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="O14" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="O14" s="19" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>6</v>
@@ -6870,7 +6878,7 @@
         <v>6</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L15" s="12" t="s">
         <v>61</v>
@@ -6882,18 +6890,18 @@
         <v>6</v>
       </c>
       <c r="O15" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>6</v>
@@ -6905,7 +6913,7 @@
         <v>17</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>4</v>
@@ -6926,21 +6934,21 @@
         <v>20</v>
       </c>
       <c r="N16" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="O16" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="O16" s="19" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>6</v>
@@ -6952,7 +6960,7 @@
         <v>17</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H17" s="10" t="s">
         <v>4</v>
@@ -6973,21 +6981,21 @@
         <v>20</v>
       </c>
       <c r="N17" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="O17" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="O17" s="19" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>6</v>
@@ -6999,7 +7007,7 @@
         <v>17</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>4</v>
@@ -7020,21 +7028,21 @@
         <v>20</v>
       </c>
       <c r="N18" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="O18" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="O18" s="19" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>6</v>
@@ -7067,10 +7075,10 @@
         <v>20</v>
       </c>
       <c r="N19" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="O19" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="O19" s="19" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -7078,10 +7086,10 @@
         <v>32</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>6</v>
@@ -7093,7 +7101,7 @@
         <v>17</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H20" s="10" t="s">
         <v>4</v>
@@ -7114,21 +7122,21 @@
         <v>20</v>
       </c>
       <c r="N20" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="O20" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="O20" s="19" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>6</v>
@@ -7152,7 +7160,7 @@
         <v>6</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L21" s="12" t="s">
         <v>61</v>
@@ -7164,7 +7172,7 @@
         <v>6</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -7172,10 +7180,10 @@
         <v>33</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>6</v>
@@ -7193,13 +7201,13 @@
         <v>20</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J22" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="K22" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="K22" s="19" t="s">
-        <v>148</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>20</v>
@@ -7216,13 +7224,13 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>6</v>
@@ -7263,13 +7271,13 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>6</v>
@@ -7310,13 +7318,13 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>6</v>
@@ -7357,13 +7365,13 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>6</v>
@@ -7399,18 +7407,18 @@
         <v>6</v>
       </c>
       <c r="O26" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>6</v>
@@ -7451,13 +7459,13 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>6</v>
@@ -7498,13 +7506,13 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>6</v>
@@ -7545,13 +7553,13 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>6</v>
@@ -7592,13 +7600,13 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>6</v>
@@ -7639,13 +7647,13 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>6</v>
@@ -7686,13 +7694,13 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>6</v>
@@ -7733,13 +7741,13 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>6</v>
@@ -7780,13 +7788,13 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>6</v>
@@ -7827,13 +7835,13 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>6</v>
@@ -7874,13 +7882,13 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>6</v>
@@ -7921,13 +7929,13 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>6</v>

</xml_diff>